<commit_message>
Solucionado error de TimeSignature y llamada a funcion
</commit_message>
<xml_diff>
--- a/Matriz_Mozart_Final.xlsx
+++ b/Matriz_Mozart_Final.xlsx
@@ -1,34 +1,93 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Omar\Claro drive\Armonia y varios\MozartDice\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8440"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Suma_Dados</t>
+  </si>
+  <si>
+    <t>Compas_1</t>
+  </si>
+  <si>
+    <t>Compas_2</t>
+  </si>
+  <si>
+    <t>Compas_3</t>
+  </si>
+  <si>
+    <t>Compas_4</t>
+  </si>
+  <si>
+    <t>Compas_5</t>
+  </si>
+  <si>
+    <t>Compas_6</t>
+  </si>
+  <si>
+    <t>Compas_7</t>
+  </si>
+  <si>
+    <t>Compas_8</t>
+  </si>
+  <si>
+    <t>Compas_9</t>
+  </si>
+  <si>
+    <t>Compas_10</t>
+  </si>
+  <si>
+    <t>Compas_11</t>
+  </si>
+  <si>
+    <t>Compas_12</t>
+  </si>
+  <si>
+    <t>Compas_13</t>
+  </si>
+  <si>
+    <t>Compas_14</t>
+  </si>
+  <si>
+    <t>Compas_15</t>
+  </si>
+  <si>
+    <t>Compas_16</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,80 +106,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,686 +408,653 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="17" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Suma_Dados</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Compas_1</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Compas_2</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Compas_3</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Compas_4</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Compas_5</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Compas_6</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Compas_7</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Compas_8</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Compas_9</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Compas_10</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Compas_11</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Compas_12</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Compas_13</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Compas_14</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Compas_15</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Compas_16</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="n">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>96</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>22</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>141</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>41</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>105</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>122</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>11</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>30</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2">
         <v>70</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2">
         <v>121</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2">
         <v>26</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2">
         <v>9</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2">
         <v>112</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2">
         <v>49</v>
       </c>
-      <c r="P2" t="n">
+      <c r="P2">
         <v>109</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2">
         <v>14</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>32</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>6</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>128</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>63</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>146</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>46</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>134</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3">
         <v>81</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J3">
         <v>117</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3">
         <v>39</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3">
         <v>126</v>
       </c>
-      <c r="M3" t="n">
+      <c r="M3">
         <v>56</v>
       </c>
-      <c r="N3" t="n">
+      <c r="N3">
         <v>174</v>
       </c>
-      <c r="O3" t="n">
+      <c r="O3">
         <v>18</v>
       </c>
-      <c r="P3" t="n">
+      <c r="P3">
         <v>116</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="Q3">
         <v>83</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>69</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>95</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>158</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>13</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>153</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>55</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>110</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4">
         <v>24</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J4">
         <v>66</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K4">
         <v>139</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L4">
         <v>15</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M4">
         <v>132</v>
       </c>
-      <c r="N4" t="n">
+      <c r="N4">
         <v>73</v>
       </c>
-      <c r="O4" t="n">
+      <c r="O4">
         <v>58</v>
       </c>
-      <c r="P4" t="n">
+      <c r="P4">
         <v>145</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="Q4">
         <v>79</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>40</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>17</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>113</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>85</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>161</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>2</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5">
         <v>159</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5">
         <v>100</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J5">
         <v>90</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K5">
         <v>176</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L5">
         <v>7</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M5">
         <v>34</v>
       </c>
-      <c r="N5" t="n">
+      <c r="N5">
         <v>67</v>
       </c>
-      <c r="O5" t="n">
+      <c r="O5">
         <v>160</v>
       </c>
-      <c r="P5" t="n">
+      <c r="P5">
         <v>52</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="Q5">
         <v>170</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>148</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>74</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>163</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>45</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>80</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>97</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>36</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6">
         <v>107</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J6">
         <v>25</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K6">
         <v>143</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L6">
         <v>64</v>
       </c>
-      <c r="M6" t="n">
+      <c r="M6">
         <v>125</v>
       </c>
-      <c r="N6" t="n">
+      <c r="N6">
         <v>76</v>
       </c>
-      <c r="O6" t="n">
+      <c r="O6">
         <v>136</v>
       </c>
-      <c r="P6" t="n">
+      <c r="P6">
         <v>1</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="Q6">
         <v>93</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>7</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>104</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>157</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>27</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>167</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>154</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>68</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>118</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7">
         <v>91</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J7">
         <v>138</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K7">
         <v>71</v>
       </c>
-      <c r="L7" t="n">
+      <c r="L7">
         <v>150</v>
       </c>
-      <c r="M7" t="n">
+      <c r="M7">
         <v>29</v>
       </c>
-      <c r="N7" t="n">
+      <c r="N7">
         <v>101</v>
       </c>
-      <c r="O7" t="n">
+      <c r="O7">
         <v>162</v>
       </c>
-      <c r="P7" t="n">
+      <c r="P7">
         <v>23</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="Q7">
         <v>151</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>152</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>60</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>171</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>53</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>99</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>133</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8">
         <v>21</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8">
         <v>127</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J8">
         <v>16</v>
       </c>
-      <c r="K8" t="n">
+      <c r="K8">
         <v>155</v>
       </c>
-      <c r="L8" t="n">
+      <c r="L8">
         <v>57</v>
       </c>
-      <c r="M8" t="n">
+      <c r="M8">
         <v>175</v>
       </c>
-      <c r="N8" t="n">
+      <c r="N8">
         <v>43</v>
       </c>
-      <c r="O8" t="n">
+      <c r="O8">
         <v>168</v>
       </c>
-      <c r="P8" t="n">
+      <c r="P8">
         <v>89</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="Q8">
         <v>172</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>119</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>84</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>114</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>50</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>140</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>86</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9">
         <v>169</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9">
         <v>94</v>
       </c>
-      <c r="J9" t="n">
+      <c r="J9">
         <v>120</v>
       </c>
-      <c r="K9" t="n">
+      <c r="K9">
         <v>88</v>
       </c>
-      <c r="L9" t="n">
+      <c r="L9">
         <v>48</v>
       </c>
-      <c r="M9" t="n">
+      <c r="M9">
         <v>166</v>
       </c>
-      <c r="N9" t="n">
+      <c r="N9">
         <v>51</v>
       </c>
-      <c r="O9" t="n">
+      <c r="O9">
         <v>115</v>
       </c>
-      <c r="P9" t="n">
+      <c r="P9">
         <v>72</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="Q9">
         <v>111</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10">
         <v>10</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>98</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>142</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>42</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>156</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>75</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>129</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10">
         <v>62</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10">
         <v>123</v>
       </c>
-      <c r="J10" t="n">
+      <c r="J10">
         <v>65</v>
       </c>
-      <c r="K10" t="n">
+      <c r="K10">
         <v>77</v>
       </c>
-      <c r="L10" t="n">
+      <c r="L10">
         <v>19</v>
       </c>
-      <c r="M10" t="n">
+      <c r="M10">
         <v>82</v>
       </c>
-      <c r="N10" t="n">
+      <c r="N10">
         <v>137</v>
       </c>
-      <c r="O10" t="n">
+      <c r="O10">
         <v>38</v>
       </c>
-      <c r="P10" t="n">
+      <c r="P10">
         <v>149</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="Q10">
         <v>8</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11">
         <v>11</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>87</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>165</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>61</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>135</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>47</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11">
         <v>147</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I11">
         <v>33</v>
       </c>
-      <c r="J11" t="n">
+      <c r="J11">
         <v>102</v>
       </c>
-      <c r="K11" t="n">
+      <c r="K11">
         <v>4</v>
       </c>
-      <c r="L11" t="n">
+      <c r="L11">
         <v>31</v>
       </c>
-      <c r="M11" t="n">
+      <c r="M11">
         <v>164</v>
       </c>
-      <c r="N11" t="n">
+      <c r="N11">
         <v>144</v>
       </c>
-      <c r="O11" t="n">
+      <c r="O11">
         <v>59</v>
       </c>
-      <c r="P11" t="n">
+      <c r="P11">
         <v>173</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="Q11">
         <v>78</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12">
         <v>12</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>54</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>130</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>10</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>103</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>28</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12">
         <v>37</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12">
         <v>106</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I12">
         <v>5</v>
       </c>
-      <c r="J12" t="n">
+      <c r="J12">
         <v>35</v>
       </c>
-      <c r="K12" t="n">
+      <c r="K12">
         <v>20</v>
       </c>
-      <c r="L12" t="n">
+      <c r="L12">
         <v>108</v>
       </c>
-      <c r="M12" t="n">
+      <c r="M12">
         <v>92</v>
       </c>
-      <c r="N12" t="n">
+      <c r="N12">
         <v>12</v>
       </c>
-      <c r="O12" t="n">
+      <c r="O12">
         <v>124</v>
       </c>
-      <c r="P12" t="n">
+      <c r="P12">
         <v>44</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="Q12">
         <v>131</v>
       </c>
     </row>

</xml_diff>